<commit_message>
added fixes to core portfolio
</commit_message>
<xml_diff>
--- a/Consumer/Dutch Bros.xlsx
+++ b/Consumer/Dutch Bros.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bina/Documents/financial-modeling/Consumer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1D299E6-FEA2-304A-A9E8-178FB6CF3684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{510F1B85-FC67-F549-8C0C-DF825FB3D738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="40960" windowHeight="22540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="2" r:id="rId1"/>
@@ -794,7 +794,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -905,12 +905,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1051,6 +1060,7 @@
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2089,8 +2099,8 @@
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>127</xdr:row>
-      <xdr:rowOff>15875</xdr:rowOff>
+      <xdr:row>126</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2125,8 +2135,7 @@
       <xxl21:absoluteUrl r:id="rId2"/>
     </xxl21:alternateUrls>
     <sheetNames>
-      <sheetName val="Factor Scoring"/>
-      <sheetName val="Factor Investing"/>
+      <sheetName val="Treasuries"/>
       <sheetName val="Hardware"/>
       <sheetName val="Software"/>
       <sheetName val="Consumer"/>
@@ -2135,21 +2144,22 @@
       <sheetName val="Industrials"/>
       <sheetName val="Real Estate"/>
       <sheetName val="Fashion + Beauty"/>
-      <sheetName val="Treasuries"/>
-      <sheetName val="All Stars"/>
-      <sheetName val="ROIC Port"/>
-      <sheetName val="To Be Modeled"/>
-      <sheetName val="My Holdings"/>
       <sheetName val="My Stocks"/>
+      <sheetName val="Compounders"/>
+      <sheetName val="GARP"/>
+      <sheetName val="Value"/>
+      <sheetName val="Aggressive Growth"/>
+      <sheetName val="Other"/>
       <sheetName val="Short List"/>
-      <sheetName val="Stable Growth"/>
-      <sheetName val="High Growth"/>
-      <sheetName val="Small Caps"/>
-      <sheetName val="Compounders"/>
-      <sheetName val="Private Companies"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
+      <sheetData sheetId="0">
+        <row r="8">
+          <cell r="C8">
+            <v>4.0480000000000002E-2</v>
+          </cell>
+        </row>
+      </sheetData>
       <sheetData sheetId="1"/>
       <sheetData sheetId="2"/>
       <sheetData sheetId="3"/>
@@ -2159,24 +2169,12 @@
       <sheetData sheetId="7"/>
       <sheetData sheetId="8"/>
       <sheetData sheetId="9"/>
-      <sheetData sheetId="10">
-        <row r="8">
-          <cell r="C8">
-            <v>4.0410000000000001E-2</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="10"/>
       <sheetData sheetId="11"/>
       <sheetData sheetId="12"/>
       <sheetData sheetId="13"/>
       <sheetData sheetId="14"/>
       <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2305,10 +2303,8 @@
     <v>54.18</v>
     <v>25.451000000000001</v>
     <v>2.327</v>
-    <v>-0.18</v>
-    <v>-6.3739999999999995E-3</v>
-    <v>0.15</v>
-    <v>5.3460000000000001E-3</v>
+    <v>1.02</v>
+    <v>3.6351000000000001E-2</v>
     <v>USD</v>
     <v>Dutch Bros Inc. is an operator and franchisor of drive-thru shops that focuses on serving hand-crafted beverages. The Company operates through two segments: Company-operated shops and Franchising and other. The Company-operated shops segment includes coffee shop sales to customers. The Franchising and other segment includes bean and product sales to franchise partners and includes the initial franchise fees, royalties, and marketing fees. The Company sells a range of customizable hot, iced, and blended beverages. Its coffee-based beverages include its espresso-based custom drinks, cold brew, and its proprietary freeze blended beverages. Its menu mix is based upon its proprietary Blue Rebel energy drink, which is customizable with flavors and modifiers and can be served blended or over ice. It also offers a variety of teas, lemonades, sodas, and smoothies. The Company has approximately 671 shops, of which 396 were Company-operated and 275 were franchised, across 14 states.</v>
     <v>22000</v>
@@ -2316,24 +2312,23 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>110 Sw 4Th Street, GRANTS PASS, OR, 97526 US</v>
-    <v>28.62</v>
+    <v>29.1</v>
     <v>Hotels &amp; Entertainment Services</v>
     <v>Stock</v>
-    <v>45114.999027060156</v>
+    <v>45117.990197707812</v>
     <v>0</v>
-    <v>28.045000000000002</v>
-    <v>4597154000</v>
+    <v>28.04</v>
+    <v>4764263640</v>
     <v>Dutch Bros Inc</v>
     <v>Dutch Bros Inc</v>
-    <v>28.21</v>
-    <v>28.24</v>
     <v>28.06</v>
-    <v>28.21</v>
+    <v>28.06</v>
+    <v>29.08</v>
     <v>163833000</v>
     <v>BROS</v>
     <v>Dutch Bros Inc (XNYS:BROS)</v>
-    <v>475439</v>
-    <v>659983</v>
+    <v>910014</v>
+    <v>659686</v>
     <v>2021</v>
   </rv>
   <rv s="2">
@@ -2365,8 +2360,6 @@
     <k n="Beta"/>
     <k n="Change"/>
     <k n="Change (%)"/>
-    <k n="Change (Extended hours)"/>
-    <k n="Change % (Extended hours)"/>
     <k n="Currency" t="s"/>
     <k n="Description" t="s"/>
     <k n="Employees"/>
@@ -2386,7 +2379,6 @@
     <k n="Open"/>
     <k n="Previous close"/>
     <k n="Price"/>
-    <k n="Price (Extended hours)"/>
     <k n="Shares outstanding"/>
     <k n="Ticker symbol" t="s"/>
     <k n="UniqueName" t="s"/>
@@ -2403,7 +2395,7 @@
 <file path=xl/richData/rdsupportingpropertybag.xml><?xml version="1.0" encoding="utf-8"?>
 <supportingPropertyBags xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2">
   <spbArrays count="1">
-    <a count="44">
+    <a count="41">
       <v t="s">%EntityServiceId</v>
       <v t="s">_Format</v>
       <v t="s">%IsRefreshable</v>
@@ -2414,16 +2406,13 @@
       <v t="s">Name</v>
       <v t="s">_SubLabel</v>
       <v t="s">Price</v>
-      <v t="s">Price (Extended hours)</v>
       <v t="s">Exchange</v>
       <v t="s">Official name</v>
       <v t="s">Last trade time</v>
       <v t="s">Ticker symbol</v>
       <v t="s">Exchange abbreviation</v>
       <v t="s">Change</v>
-      <v t="s">Change (Extended hours)</v>
       <v t="s">Change (%)</v>
-      <v t="s">Change % (Extended hours)</v>
       <v t="s">Currency</v>
       <v t="s">Previous close</v>
       <v t="s">Open</v>
@@ -2487,19 +2476,13 @@
       <v>8</v>
       <v>9</v>
       <v>4</v>
-      <v>1</v>
-      <v>1</v>
-      <v>5</v>
     </spb>
     <spb s="4">
-      <v>at close</v>
+      <v>Delayed 15 minutes</v>
       <v>from previous close</v>
       <v>from previous close</v>
       <v>Source: Nasdaq</v>
       <v>GMT</v>
-      <v>Delayed 15 minutes</v>
-      <v>from close</v>
-      <v>from close</v>
     </spb>
   </spbData>
 </supportingPropertyBags>
@@ -2543,9 +2526,6 @@
     <k n="Year incorporated" t="i"/>
     <k n="`%EntityServiceId" t="i"/>
     <k n="Shares outstanding" t="i"/>
-    <k n="Price (Extended hours)" t="i"/>
-    <k n="Change (Extended hours)" t="i"/>
-    <k n="Change % (Extended hours)" t="i"/>
   </s>
   <s>
     <k n="Price" t="s"/>
@@ -2553,9 +2533,6 @@
     <k n="Change (%)" t="s"/>
     <k n="ExchangeID" t="s"/>
     <k n="Last trade time" t="s"/>
-    <k n="Price (Extended hours)" t="s"/>
-    <k n="Change (Extended hours)" t="s"/>
-    <k n="Change % (Extended hours)" t="s"/>
   </s>
 </spbStructures>
 </file>
@@ -3133,10 +3110,10 @@
   <dimension ref="A1:AL119"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C89" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B67" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H102" sqref="H102"/>
+      <selection pane="bottomRight" activeCell="H89" sqref="H89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3256,10 +3233,10 @@
         <v>974300000</v>
       </c>
       <c r="G4" s="24">
-        <v>1242000000</v>
+        <v>1243000000</v>
       </c>
       <c r="H4" s="24">
-        <v>1529000000</v>
+        <v>1542000000</v>
       </c>
       <c r="I4" s="24">
         <v>1817000000</v>
@@ -3303,15 +3280,15 @@
       </c>
       <c r="G5" s="16">
         <f t="shared" si="0"/>
-        <v>0.27476136713537924</v>
+        <v>0.27578774504772663</v>
       </c>
       <c r="H5" s="16">
         <f t="shared" si="0"/>
-        <v>0.23107890499194839</v>
+        <v>0.24054706355591304</v>
       </c>
       <c r="I5" s="16">
         <f t="shared" si="0"/>
-        <v>0.18835840418574223</v>
+        <v>0.17833981841763946</v>
       </c>
       <c r="J5" s="16">
         <f t="shared" si="0"/>
@@ -3669,15 +3646,15 @@
       </c>
       <c r="L17" s="36">
         <f>M102/E4</f>
-        <v>6.2206757129789505</v>
+        <v>6.4468014592455871</v>
       </c>
       <c r="M17" s="36">
         <f>M102/E29</f>
-        <v>-967.21102461603198</v>
+        <v>-1002.3697959183673</v>
       </c>
       <c r="N17" s="37">
         <f>M102/E108</f>
-        <v>-35.916107408767395</v>
+        <v>-37.221682070673531</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="19" x14ac:dyDescent="0.25">
@@ -3746,7 +3723,7 @@
         <v>127700000</v>
       </c>
       <c r="G20" s="35">
-        <v>182800000</v>
+        <v>179400000</v>
       </c>
       <c r="H20" s="35">
         <v>226000000</v>
@@ -3763,15 +3740,15 @@
       </c>
       <c r="L20" s="36">
         <f>M102/F4</f>
-        <v>4.7184173252591606</v>
+        <v>4.8899349686954734</v>
       </c>
       <c r="M20" s="38">
         <f>G117/F32</f>
-        <v>71.948717948717942</v>
+        <v>63.217391304347821</v>
       </c>
       <c r="N20" s="37">
         <f>M102/F107</f>
-        <v>-43.699182509505704</v>
+        <v>-45.28767718631179</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -3797,11 +3774,11 @@
       </c>
       <c r="G21" s="16">
         <f t="shared" si="3"/>
-        <v>0.43148003132341417</v>
+        <v>0.40485512920908384</v>
       </c>
       <c r="H21" s="16">
         <f t="shared" si="3"/>
-        <v>0.23632385120350108</v>
+        <v>0.25975473801560756</v>
       </c>
       <c r="I21" s="16">
         <f t="shared" si="3"/>
@@ -3828,23 +3805,23 @@
       <c r="E22" s="2">
         <v>8.2000000000000003E-2</v>
       </c>
-      <c r="F22" s="42">
+      <c r="F22" s="72">
         <f>F20/F4</f>
         <v>0.13106845940675357</v>
       </c>
-      <c r="G22" s="42">
+      <c r="G22" s="72">
         <f t="shared" ref="G22:J22" si="4">G20/G4</f>
-        <v>0.14718196457326893</v>
-      </c>
-      <c r="H22" s="42">
+        <v>0.14432823813354786</v>
+      </c>
+      <c r="H22" s="72">
         <f t="shared" si="4"/>
-        <v>0.14780902550686723</v>
-      </c>
-      <c r="I22" s="42">
+        <v>0.14656290531776914</v>
+      </c>
+      <c r="I22" s="72">
         <f t="shared" si="4"/>
         <v>0.1565767749036874</v>
       </c>
-      <c r="J22" s="42">
+      <c r="J22" s="72">
         <f t="shared" si="4"/>
         <v>0.16311360448807855</v>
       </c>
@@ -3877,7 +3854,7 @@
       </c>
       <c r="N23" s="46">
         <f>E108/M102</f>
-        <v>-2.784266091586229E-2</v>
+        <v>-2.6866061509559953E-2</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="19" x14ac:dyDescent="0.25">
@@ -3982,19 +3959,19 @@
         <v>-4753000</v>
       </c>
       <c r="F29" s="40">
-        <v>22780000</v>
+        <v>27000000</v>
       </c>
       <c r="G29" s="40">
-        <v>78490000</v>
+        <v>49000000</v>
       </c>
       <c r="H29" s="40">
-        <v>70495000</v>
+        <v>62000000</v>
       </c>
       <c r="I29" s="40">
-        <v>107000000</v>
+        <v>92000000</v>
       </c>
       <c r="J29" s="40">
-        <v>149100000</v>
+        <v>118000000</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="20" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -4016,23 +3993,23 @@
       </c>
       <c r="F30" s="16">
         <f t="shared" ref="F30:J30" si="5">(F29/E29)-1</f>
-        <v>-5.7927624658110668</v>
+        <v>-6.6806227645697458</v>
       </c>
       <c r="G30" s="16">
         <f t="shared" si="5"/>
-        <v>2.4455662862159788</v>
+        <v>0.81481481481481488</v>
       </c>
       <c r="H30" s="16">
         <f t="shared" si="5"/>
-        <v>-0.10186010956809788</v>
+        <v>0.26530612244897966</v>
       </c>
       <c r="I30" s="16">
         <f t="shared" si="5"/>
-        <v>0.51783814454925881</v>
+        <v>0.4838709677419355</v>
       </c>
       <c r="J30" s="16">
         <f t="shared" si="5"/>
-        <v>0.3934579439252337</v>
+        <v>0.28260869565217384</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="19" x14ac:dyDescent="0.25">
@@ -4053,23 +4030,23 @@
       </c>
       <c r="F31" s="42">
         <f>F29/F4</f>
-        <v>2.3380888843272093E-2</v>
+        <v>2.771220363337781E-2</v>
       </c>
       <c r="G31" s="42">
         <f t="shared" ref="G31:J31" si="6">G29/G4</f>
-        <v>6.3196457326892108E-2</v>
+        <v>3.9420756234915526E-2</v>
       </c>
       <c r="H31" s="42">
         <f t="shared" si="6"/>
-        <v>4.6105297580117721E-2</v>
+        <v>4.0207522697795074E-2</v>
       </c>
       <c r="I31" s="42">
         <f t="shared" si="6"/>
-        <v>5.8888277380297192E-2</v>
+        <v>5.0632911392405063E-2</v>
       </c>
       <c r="J31" s="42">
         <f t="shared" si="6"/>
-        <v>6.9705469845722304E-2</v>
+        <v>5.5165965404394578E-2</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="19" x14ac:dyDescent="0.25">
@@ -4089,19 +4066,19 @@
         <v>-0.09</v>
       </c>
       <c r="F32" s="41">
-        <v>0.39</v>
+        <v>0.46</v>
       </c>
       <c r="G32" s="41">
-        <v>1.35</v>
+        <v>0.85</v>
       </c>
       <c r="H32" s="41">
-        <v>1.21</v>
+        <v>1.07</v>
       </c>
       <c r="I32" s="41">
-        <v>1.84</v>
+        <v>1.59</v>
       </c>
       <c r="J32" s="41">
-        <v>2.57</v>
+        <v>2.02</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="19" x14ac:dyDescent="0.25">
@@ -5256,7 +5233,7 @@
       </c>
       <c r="M95" s="51">
         <f>[1]Treasuries!$C$8</f>
-        <v>4.0410000000000001E-2</v>
+        <v>4.0480000000000002E-2</v>
       </c>
     </row>
     <row r="96" spans="1:13" ht="20" x14ac:dyDescent="0.25">
@@ -5327,7 +5304,7 @@
       </c>
       <c r="M98" s="50">
         <f>(M95)+((M96)*(M97-M95))</f>
-        <v>0.14184393000000001</v>
+        <v>0.14175103999999999</v>
       </c>
     </row>
     <row r="99" spans="1:13" ht="19" x14ac:dyDescent="0.25">
@@ -5396,7 +5373,7 @@
       </c>
       <c r="M101" s="50">
         <f>M100/M104</f>
-        <v>0.11975270417577856</v>
+        <v>0.11603971399685752</v>
       </c>
     </row>
     <row r="102" spans="1:13" ht="20" x14ac:dyDescent="0.25">
@@ -5420,7 +5397,7 @@
       </c>
       <c r="M102" s="53" cm="1">
         <f t="array" ref="M102">_FV(A1,"Market cap",TRUE)</f>
-        <v>4597154000</v>
+        <v>4764263640</v>
       </c>
     </row>
     <row r="103" spans="1:13" ht="20" x14ac:dyDescent="0.25">
@@ -5444,7 +5421,7 @@
       </c>
       <c r="M103" s="50">
         <f>M102/M104</f>
-        <v>0.88024729582422145</v>
+        <v>0.88396028600314247</v>
       </c>
     </row>
     <row r="104" spans="1:13" ht="20" x14ac:dyDescent="0.25">
@@ -5468,7 +5445,7 @@
       </c>
       <c r="M104" s="54">
         <f>M100+M102</f>
-        <v>5222571000</v>
+        <v>5389680640</v>
       </c>
     </row>
     <row r="105" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.3">
@@ -5514,23 +5491,23 @@
       </c>
       <c r="F106" s="32">
         <f>E106*(1+$M$107)</f>
-        <v>-190111652.16279703</v>
+        <v>-190126270.37958276</v>
       </c>
       <c r="G106" s="32">
         <f t="shared" ref="G106:J106" si="11">F106*(1+$M$107)</f>
-        <v>-235350457.63305995</v>
+        <v>-235386652.53476432</v>
       </c>
       <c r="H106" s="32">
         <f t="shared" si="11"/>
-        <v>-291354250.39943969</v>
+        <v>-291421464.69766283</v>
       </c>
       <c r="I106" s="32">
         <f t="shared" si="11"/>
-        <v>-360684657.59335405</v>
+        <v>-360795606.59875703</v>
       </c>
       <c r="J106" s="32">
         <f t="shared" si="11"/>
-        <v>-446512868.93834597</v>
+        <v>-446684563.45868134</v>
       </c>
       <c r="K106" s="33" t="s">
         <v>172</v>
@@ -5540,7 +5517,7 @@
       </c>
       <c r="M106" s="56">
         <f>(M101*M93)+(M103*M98)</f>
-        <v>0.12884616678486743</v>
+        <v>0.129167057612671</v>
       </c>
     </row>
     <row r="107" spans="1:13" ht="19" x14ac:dyDescent="0.25">
@@ -5564,7 +5541,7 @@
         <v>-105200000</v>
       </c>
       <c r="G107" s="43">
-        <v>-66125000</v>
+        <v>-70000000</v>
       </c>
       <c r="H107" s="43">
         <v>5000000</v>
@@ -5583,7 +5560,7 @@
       </c>
       <c r="M107" s="58">
         <f>(SUM(F5:J5)/5)</f>
-        <v>0.23795914114471986</v>
+        <v>0.23805433128636172</v>
       </c>
     </row>
     <row r="108" spans="1:13" ht="19" x14ac:dyDescent="0.25">
@@ -5608,7 +5585,7 @@
       <c r="I108" s="33"/>
       <c r="J108" s="44">
         <f>J107*(1+M108)/(M109-M108)</f>
-        <v>2467592285.1428828</v>
+        <v>2459990767.4538116</v>
       </c>
       <c r="K108" s="34" t="s">
         <v>157</v>
@@ -5627,7 +5604,7 @@
       </c>
       <c r="G109" s="44">
         <f t="shared" si="12"/>
-        <v>-66125000</v>
+        <v>-70000000</v>
       </c>
       <c r="H109" s="44">
         <f t="shared" si="12"/>
@@ -5639,7 +5616,7 @@
       </c>
       <c r="J109" s="44">
         <f>J108+J107</f>
-        <v>2717592285.1428828</v>
+        <v>2709990767.4538116</v>
       </c>
       <c r="K109" s="34" t="s">
         <v>153</v>
@@ -5649,7 +5626,7 @@
       </c>
       <c r="M109" s="58">
         <f>M106</f>
-        <v>0.12884616678486743</v>
+        <v>0.129167057612671</v>
       </c>
     </row>
     <row r="110" spans="1:13" ht="19" x14ac:dyDescent="0.25">
@@ -5664,7 +5641,7 @@
       </c>
       <c r="G111" s="53">
         <f>NPV(M109,F109,G109,H109,I109,J109)</f>
-        <v>1433320302.7832096</v>
+        <v>1423982750.6084766</v>
       </c>
     </row>
     <row r="112" spans="1:13" ht="20" x14ac:dyDescent="0.25">
@@ -5691,7 +5668,7 @@
       </c>
       <c r="G114" s="53">
         <f>G111+G112-G113</f>
-        <v>828081302.78320956</v>
+        <v>818743750.60847664</v>
       </c>
     </row>
     <row r="115" spans="6:7" ht="20" x14ac:dyDescent="0.25">
@@ -5709,7 +5686,7 @@
       </c>
       <c r="G116" s="64">
         <f>G114/G115</f>
-        <v>13.49901890750607</v>
+        <v>13.346802219443083</v>
       </c>
     </row>
     <row r="117" spans="6:7" ht="20" x14ac:dyDescent="0.25">
@@ -5718,7 +5695,7 @@
       </c>
       <c r="G117" s="65" cm="1">
         <f t="array" ref="G117">_FV(A1,"Price")</f>
-        <v>28.06</v>
+        <v>29.08</v>
       </c>
     </row>
     <row r="118" spans="6:7" ht="20" x14ac:dyDescent="0.25">
@@ -5727,7 +5704,7 @@
       </c>
       <c r="G118" s="66">
         <f>G116/G117-1</f>
-        <v>-0.51892306102971952</v>
+        <v>-0.5410315605418472</v>
       </c>
     </row>
     <row r="119" spans="6:7" ht="20" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated many models and dashboard (hardware + software)
</commit_message>
<xml_diff>
--- a/Consumer/Dutch Bros.xlsx
+++ b/Consumer/Dutch Bros.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bina/Documents/financial-modeling/Consumer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{510F1B85-FC67-F549-8C0C-DF825FB3D738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48CACF47-EA52-814A-8E32-703DABD986A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="40960" windowHeight="22540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="2" r:id="rId1"/>
@@ -1048,6 +1048,7 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1060,7 +1061,6 @@
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2145,6 +2145,7 @@
       <sheetName val="Real Estate"/>
       <sheetName val="Fashion + Beauty"/>
       <sheetName val="My Stocks"/>
+      <sheetName val="Profitable Software"/>
       <sheetName val="Compounders"/>
       <sheetName val="GARP"/>
       <sheetName val="Value"/>
@@ -2156,7 +2157,7 @@
       <sheetData sheetId="0">
         <row r="8">
           <cell r="C8">
-            <v>4.0480000000000002E-2</v>
+            <v>3.9120000000000002E-2</v>
           </cell>
         </row>
       </sheetData>
@@ -2175,6 +2176,7 @@
       <sheetData sheetId="13"/>
       <sheetData sheetId="14"/>
       <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2302,9 +2304,11 @@
     <v>Powered by Refinitiv</v>
     <v>54.18</v>
     <v>25.451000000000001</v>
-    <v>2.327</v>
-    <v>1.02</v>
-    <v>3.6351000000000001E-2</v>
+    <v>2.298</v>
+    <v>0.44</v>
+    <v>1.5443999999999999E-2</v>
+    <v>7.0000000000000007E-2</v>
+    <v>2.4199999999999998E-3</v>
     <v>USD</v>
     <v>Dutch Bros Inc. is an operator and franchisor of drive-thru shops that focuses on serving hand-crafted beverages. The Company operates through two segments: Company-operated shops and Franchising and other. The Company-operated shops segment includes coffee shop sales to customers. The Franchising and other segment includes bean and product sales to franchise partners and includes the initial franchise fees, royalties, and marketing fees. The Company sells a range of customizable hot, iced, and blended beverages. Its coffee-based beverages include its espresso-based custom drinks, cold brew, and its proprietary freeze blended beverages. Its menu mix is based upon its proprietary Blue Rebel energy drink, which is customizable with flavors and modifiers and can be served blended or over ice. It also offers a variety of teas, lemonades, sodas, and smoothies. The Company has approximately 671 shops, of which 396 were Company-operated and 275 were franchised, across 14 states.</v>
     <v>22000</v>
@@ -2312,23 +2316,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>110 Sw 4Th Street, GRANTS PASS, OR, 97526 US</v>
-    <v>29.1</v>
+    <v>29.26</v>
     <v>Hotels &amp; Entertainment Services</v>
     <v>Stock</v>
-    <v>45117.990197707812</v>
+    <v>45132.966239363283</v>
     <v>0</v>
-    <v>28.04</v>
-    <v>4764263640</v>
+    <v>28.49</v>
+    <v>4739688690</v>
     <v>Dutch Bros Inc</v>
     <v>Dutch Bros Inc</v>
-    <v>28.06</v>
-    <v>28.06</v>
-    <v>29.08</v>
+    <v>28.49</v>
+    <v>28.49</v>
+    <v>28.93</v>
+    <v>29</v>
     <v>163833000</v>
     <v>BROS</v>
     <v>Dutch Bros Inc (XNYS:BROS)</v>
-    <v>910014</v>
-    <v>659686</v>
+    <v>612952</v>
+    <v>606220</v>
     <v>2021</v>
   </rv>
   <rv s="2">
@@ -2360,6 +2365,8 @@
     <k n="Beta"/>
     <k n="Change"/>
     <k n="Change (%)"/>
+    <k n="Change (Extended hours)"/>
+    <k n="Change % (Extended hours)"/>
     <k n="Currency" t="s"/>
     <k n="Description" t="s"/>
     <k n="Employees"/>
@@ -2379,6 +2386,7 @@
     <k n="Open"/>
     <k n="Previous close"/>
     <k n="Price"/>
+    <k n="Price (Extended hours)"/>
     <k n="Shares outstanding"/>
     <k n="Ticker symbol" t="s"/>
     <k n="UniqueName" t="s"/>
@@ -2395,7 +2403,7 @@
 <file path=xl/richData/rdsupportingpropertybag.xml><?xml version="1.0" encoding="utf-8"?>
 <supportingPropertyBags xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2">
   <spbArrays count="1">
-    <a count="41">
+    <a count="44">
       <v t="s">%EntityServiceId</v>
       <v t="s">_Format</v>
       <v t="s">%IsRefreshable</v>
@@ -2406,13 +2414,16 @@
       <v t="s">Name</v>
       <v t="s">_SubLabel</v>
       <v t="s">Price</v>
+      <v t="s">Price (Extended hours)</v>
       <v t="s">Exchange</v>
       <v t="s">Official name</v>
       <v t="s">Last trade time</v>
       <v t="s">Ticker symbol</v>
       <v t="s">Exchange abbreviation</v>
       <v t="s">Change</v>
+      <v t="s">Change (Extended hours)</v>
       <v t="s">Change (%)</v>
+      <v t="s">Change % (Extended hours)</v>
       <v t="s">Currency</v>
       <v t="s">Previous close</v>
       <v t="s">Open</v>
@@ -2476,13 +2487,19 @@
       <v>8</v>
       <v>9</v>
       <v>4</v>
+      <v>1</v>
+      <v>1</v>
+      <v>5</v>
     </spb>
     <spb s="4">
-      <v>Delayed 15 minutes</v>
+      <v>at close</v>
       <v>from previous close</v>
       <v>from previous close</v>
       <v>Source: Nasdaq</v>
       <v>GMT</v>
+      <v>Delayed 15 minutes</v>
+      <v>from close</v>
+      <v>from close</v>
     </spb>
   </spbData>
 </supportingPropertyBags>
@@ -2526,6 +2543,9 @@
     <k n="Year incorporated" t="i"/>
     <k n="`%EntityServiceId" t="i"/>
     <k n="Shares outstanding" t="i"/>
+    <k n="Price (Extended hours)" t="i"/>
+    <k n="Change (Extended hours)" t="i"/>
+    <k n="Change % (Extended hours)" t="i"/>
   </s>
   <s>
     <k n="Price" t="s"/>
@@ -2533,6 +2553,9 @@
     <k n="Change (%)" t="s"/>
     <k n="ExchangeID" t="s"/>
     <k n="Last trade time" t="s"/>
+    <k n="Price (Extended hours)" t="s"/>
+    <k n="Change (Extended hours)" t="s"/>
+    <k n="Change % (Extended hours)" t="s"/>
   </s>
 </spbStructures>
 </file>
@@ -3110,10 +3133,10 @@
   <dimension ref="A1:AL119"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B67" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B98" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H89" sqref="H89"/>
+      <selection pane="bottomRight" activeCell="C125" sqref="C125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3646,15 +3669,15 @@
       </c>
       <c r="L17" s="36">
         <f>M102/E4</f>
-        <v>6.4468014592455871</v>
+        <v>6.413547669050029</v>
       </c>
       <c r="M17" s="36">
         <f>M102/E29</f>
-        <v>-1002.3697959183673</v>
+        <v>-997.19938775510207</v>
       </c>
       <c r="N17" s="37">
         <f>M102/E108</f>
-        <v>-37.221682070673531</v>
+        <v>-37.029685773885326</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="19" x14ac:dyDescent="0.25">
@@ -3740,15 +3763,15 @@
       </c>
       <c r="L20" s="36">
         <f>M102/F4</f>
-        <v>4.8899349686954734</v>
+        <v>4.8647117828184339</v>
       </c>
       <c r="M20" s="38">
         <f>G117/F32</f>
-        <v>63.217391304347821</v>
+        <v>62.891304347826086</v>
       </c>
       <c r="N20" s="37">
         <f>M102/F107</f>
-        <v>-45.28767718631179</v>
+        <v>-45.054074999999997</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -3805,23 +3828,23 @@
       <c r="E22" s="2">
         <v>8.2000000000000003E-2</v>
       </c>
-      <c r="F22" s="72">
+      <c r="F22" s="68">
         <f>F20/F4</f>
         <v>0.13106845940675357</v>
       </c>
-      <c r="G22" s="72">
+      <c r="G22" s="68">
         <f t="shared" ref="G22:J22" si="4">G20/G4</f>
         <v>0.14432823813354786</v>
       </c>
-      <c r="H22" s="72">
+      <c r="H22" s="68">
         <f t="shared" si="4"/>
         <v>0.14656290531776914</v>
       </c>
-      <c r="I22" s="72">
+      <c r="I22" s="68">
         <f t="shared" si="4"/>
         <v>0.1565767749036874</v>
       </c>
-      <c r="J22" s="72">
+      <c r="J22" s="68">
         <f t="shared" si="4"/>
         <v>0.16311360448807855</v>
       </c>
@@ -3854,7 +3877,7 @@
       </c>
       <c r="N23" s="46">
         <f>E108/M102</f>
-        <v>-2.6866061509559953E-2</v>
+        <v>-2.7005360134739146E-2</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="19" x14ac:dyDescent="0.25">
@@ -4969,10 +4992,10 @@
       <c r="E84" s="1">
         <v>-15817000</v>
       </c>
-      <c r="L84" s="69" t="s">
+      <c r="L84" s="70" t="s">
         <v>134</v>
       </c>
-      <c r="M84" s="70"/>
+      <c r="M84" s="71"/>
     </row>
     <row r="85" spans="1:13" ht="19" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
@@ -4990,10 +5013,10 @@
       <c r="E85" s="1">
         <v>1606000</v>
       </c>
-      <c r="L85" s="71" t="s">
+      <c r="L85" s="72" t="s">
         <v>135</v>
       </c>
-      <c r="M85" s="71"/>
+      <c r="M85" s="72"/>
     </row>
     <row r="86" spans="1:13" ht="20" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
@@ -5207,10 +5230,10 @@
       <c r="E94" s="1">
         <v>-4692000</v>
       </c>
-      <c r="L94" s="71" t="s">
+      <c r="L94" s="72" t="s">
         <v>143</v>
       </c>
-      <c r="M94" s="71"/>
+      <c r="M94" s="72"/>
     </row>
     <row r="95" spans="1:13" ht="20" x14ac:dyDescent="0.25">
       <c r="A95" s="6" t="s">
@@ -5233,7 +5256,7 @@
       </c>
       <c r="M95" s="51">
         <f>[1]Treasuries!$C$8</f>
-        <v>4.0480000000000002E-2</v>
+        <v>3.9120000000000002E-2</v>
       </c>
     </row>
     <row r="96" spans="1:13" ht="20" x14ac:dyDescent="0.25">
@@ -5257,7 +5280,7 @@
       </c>
       <c r="M96" s="52" cm="1">
         <f t="array" ref="M96">_FV(A1,"Beta")</f>
-        <v>2.327</v>
+        <v>2.298</v>
       </c>
     </row>
     <row r="97" spans="1:13" ht="20" x14ac:dyDescent="0.25">
@@ -5304,7 +5327,7 @@
       </c>
       <c r="M98" s="50">
         <f>(M95)+((M96)*(M97-M95))</f>
-        <v>0.14175103999999999</v>
+        <v>0.14225424000000003</v>
       </c>
     </row>
     <row r="99" spans="1:13" ht="19" x14ac:dyDescent="0.25">
@@ -5323,10 +5346,10 @@
       <c r="E99" s="1">
         <v>0</v>
       </c>
-      <c r="L99" s="71" t="s">
+      <c r="L99" s="72" t="s">
         <v>148</v>
       </c>
-      <c r="M99" s="71"/>
+      <c r="M99" s="72"/>
     </row>
     <row r="100" spans="1:13" ht="20" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
@@ -5373,7 +5396,7 @@
       </c>
       <c r="M101" s="50">
         <f>M100/M104</f>
-        <v>0.11603971399685752</v>
+        <v>0.11657123571036306</v>
       </c>
     </row>
     <row r="102" spans="1:13" ht="20" x14ac:dyDescent="0.25">
@@ -5397,7 +5420,7 @@
       </c>
       <c r="M102" s="53" cm="1">
         <f t="array" ref="M102">_FV(A1,"Market cap",TRUE)</f>
-        <v>4764263640</v>
+        <v>4739688690</v>
       </c>
     </row>
     <row r="103" spans="1:13" ht="20" x14ac:dyDescent="0.25">
@@ -5421,7 +5444,7 @@
       </c>
       <c r="M103" s="50">
         <f>M102/M104</f>
-        <v>0.88396028600314247</v>
+        <v>0.8834287642896369</v>
       </c>
     </row>
     <row r="104" spans="1:13" ht="20" x14ac:dyDescent="0.25">
@@ -5445,7 +5468,7 @@
       </c>
       <c r="M104" s="54">
         <f>M100+M102</f>
-        <v>5389680640</v>
+        <v>5365105690</v>
       </c>
     </row>
     <row r="105" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.3">
@@ -5464,10 +5487,10 @@
       <c r="E105" s="11">
         <v>20178000</v>
       </c>
-      <c r="L105" s="71" t="s">
+      <c r="L105" s="72" t="s">
         <v>154</v>
       </c>
-      <c r="M105" s="71"/>
+      <c r="M105" s="72"/>
     </row>
     <row r="106" spans="1:13" ht="21" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A106" s="14" t="s">
@@ -5517,7 +5540,7 @@
       </c>
       <c r="M106" s="56">
         <f>(M101*M93)+(M103*M98)</f>
-        <v>0.129167057612671</v>
+        <v>0.12955395783995033</v>
       </c>
     </row>
     <row r="107" spans="1:13" ht="19" x14ac:dyDescent="0.25">
@@ -5585,7 +5608,7 @@
       <c r="I108" s="33"/>
       <c r="J108" s="44">
         <f>J107*(1+M108)/(M109-M108)</f>
-        <v>2459990767.4538116</v>
+        <v>2450887611.4691296</v>
       </c>
       <c r="K108" s="34" t="s">
         <v>157</v>
@@ -5616,7 +5639,7 @@
       </c>
       <c r="J109" s="44">
         <f>J108+J107</f>
-        <v>2709990767.4538116</v>
+        <v>2700887611.4691296</v>
       </c>
       <c r="K109" s="34" t="s">
         <v>153</v>
@@ -5626,14 +5649,14 @@
       </c>
       <c r="M109" s="58">
         <f>M106</f>
-        <v>0.129167057612671</v>
+        <v>0.12955395783995033</v>
       </c>
     </row>
     <row r="110" spans="1:13" ht="19" x14ac:dyDescent="0.25">
-      <c r="F110" s="68" t="s">
+      <c r="F110" s="69" t="s">
         <v>160</v>
       </c>
-      <c r="G110" s="68"/>
+      <c r="G110" s="69"/>
     </row>
     <row r="111" spans="1:13" ht="20" x14ac:dyDescent="0.25">
       <c r="F111" s="62" t="s">
@@ -5641,7 +5664,7 @@
       </c>
       <c r="G111" s="53">
         <f>NPV(M109,F109,G109,H109,I109,J109)</f>
-        <v>1423982750.6084766</v>
+        <v>1416445125.5442755</v>
       </c>
     </row>
     <row r="112" spans="1:13" ht="20" x14ac:dyDescent="0.25">
@@ -5668,7 +5691,7 @@
       </c>
       <c r="G114" s="53">
         <f>G111+G112-G113</f>
-        <v>818743750.60847664</v>
+        <v>811206125.54427552</v>
       </c>
     </row>
     <row r="115" spans="6:7" ht="20" x14ac:dyDescent="0.25">
@@ -5686,7 +5709,7 @@
       </c>
       <c r="G116" s="64">
         <f>G114/G115</f>
-        <v>13.346802219443083</v>
+        <v>13.22392715522251</v>
       </c>
     </row>
     <row r="117" spans="6:7" ht="20" x14ac:dyDescent="0.25">
@@ -5695,7 +5718,7 @@
       </c>
       <c r="G117" s="65" cm="1">
         <f t="array" ref="G117">_FV(A1,"Price")</f>
-        <v>29.08</v>
+        <v>28.93</v>
       </c>
     </row>
     <row r="118" spans="6:7" ht="20" x14ac:dyDescent="0.25">
@@ -5704,7 +5727,7 @@
       </c>
       <c r="G118" s="66">
         <f>G116/G117-1</f>
-        <v>-0.5410315605418472</v>
+        <v>-0.54289916504588631</v>
       </c>
     </row>
     <row r="119" spans="6:7" ht="20" x14ac:dyDescent="0.25">

</xml_diff>